<commit_message>
Se eliminan duplicados en Veterinarios.xlsx
</commit_message>
<xml_diff>
--- a/pet/src/main/resources/Veterinarios.xlsx
+++ b/pet/src/main/resources/Veterinarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BEDU\BEDU-Equipo19\pet\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Archivos\03_Habilidades\2023_Beca-Santander\Codigo\Java\06_Java-Backend-II\Proyecto\202312_13\BEDU-Equipo19\pet\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1148A8F3-542A-4FF9-95CD-5AF0A1C5F860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{618AEDA0-C773-49F9-868F-6BC094E97661}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18510" yWindow="3720" windowWidth="21600" windowHeight="11205" xr2:uid="{E48F61DF-3797-46C9-90F0-8B7283C32CBA}"/>
+    <workbookView xWindow="5115" yWindow="555" windowWidth="15375" windowHeight="7785" xr2:uid="{E48F61DF-3797-46C9-90F0-8B7283C32CBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -53,30 +53,6 @@
     <t>Telefono</t>
   </si>
   <si>
-    <t>luis</t>
-  </si>
-  <si>
-    <t>ignacio</t>
-  </si>
-  <si>
-    <t>castro</t>
-  </si>
-  <si>
-    <t>jairbuny@gmail.com</t>
-  </si>
-  <si>
-    <t>sharon</t>
-  </si>
-  <si>
-    <t>estrada</t>
-  </si>
-  <si>
-    <t>martinez</t>
-  </si>
-  <si>
-    <t>sharon@gmail.com</t>
-  </si>
-  <si>
     <t>Cedula</t>
   </si>
   <si>
@@ -87,6 +63,30 @@
   </si>
   <si>
     <t>odontologia</t>
+  </si>
+  <si>
+    <t>Joaquin</t>
+  </si>
+  <si>
+    <t>Sosa</t>
+  </si>
+  <si>
+    <t>Estrada</t>
+  </si>
+  <si>
+    <t>sosa-je@gmail.com</t>
+  </si>
+  <si>
+    <t>Matha</t>
+  </si>
+  <si>
+    <t>Pastrana</t>
+  </si>
+  <si>
+    <t>Rios</t>
+  </si>
+  <si>
+    <t>rios-mpast@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -136,7 +136,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -452,10 +452,10 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -474,56 +474,56 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E2">
         <v>8121495228</v>
       </c>
       <c r="F2">
-        <v>12345678</v>
+        <v>56781234</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E3">
         <v>8521495228</v>
       </c>
       <c r="F3">
-        <v>87654321</v>
+        <v>21876543</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>